<commit_message>
Completed rectangle.py file and did unittesting
</commit_message>
<xml_diff>
--- a/tests/test_plan_rectangle.xlsx
+++ b/tests/test_plan_rectangle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\8. Activities\Module_02\given_files\activity_2\activity_2\tests\shape\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rrcca-my.sharepoint.com/personal/nsidhu10_rrc_ca/Documents/Desktop/rrc_polytech/Intermediate Software Developement/Activities/Activity_02/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D0B001-6057-4615-9964-5A71A3F0CEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{75D0B001-6057-4615-9964-5A71A3F0CEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F703CAAC-AAB5-484B-9A96-52D9CDAA3EE5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,9 +161,10 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
-  <metadataTypes count="1">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLRICHVALUE" count="1">
     <bk>
@@ -174,6 +175,20 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </cellMetadata>
   <valueMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
@@ -183,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -246,13 +261,58 @@
   </si>
   <si>
     <t>Rectangle</t>
+  </si>
+  <si>
+    <t>Navkaran Singh Sidhu</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Rectangle("Green",9,10)</t>
+  </si>
+  <si>
+    <t>Attribute set to argument value.</t>
+  </si>
+  <si>
+    <t>ValueError</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>The shape color is green.This rectangle has four sides with the lengths of 9, 10, 9 and 10 centimeters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Rectangle("",9,10)</t>
+  </si>
+  <si>
+    <t>Rectangle("Green","Nine",10)</t>
+  </si>
+  <si>
+    <t>Rectangle("Green",9,"Ten")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +373,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -500,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -550,12 +623,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -780,8 +857,10 @@
     <tableColumn id="2" xr3:uid="{1904C92F-9639-4229-AA4E-4C4DEAF21EEE}" name="Method being Tested" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{4E480EB6-99FB-4F51-98B5-D5BE13327E8C}" name="Condition being Tested" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{5381561B-09C5-439D-999E-CD8E013F9561}" name="Preconditions" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{645704DE-22F5-4239-BEB6-F4252A1F2823}" name="Method Inputs" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{101F480E-86C3-4E60-AA1E-2FCAD389E35F}" name="Expected Result" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{645704DE-22F5-4239-BEB6-F4252A1F2823}" name="Method Inputs" dataDxfId="0">
+      <calculatedColumnFormula array="1">F5:F7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{101F480E-86C3-4E60-AA1E-2FCAD389E35F}" name="Expected Result" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1106,22 +1185,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" customWidth="1"/>
+    <col min="6" max="6" width="35.453125" customWidth="1"/>
+    <col min="7" max="7" width="26.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="2.15">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1133,14 +1212,16 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1149,10 +1230,10 @@
       </c>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="11">
         <v>1</v>
@@ -1183,11 +1264,17 @@
       <c r="D7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="12">
         <v>2</v>
@@ -1198,11 +1285,17 @@
       <c r="D8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="12">
         <v>3</v>
@@ -1213,11 +1306,17 @@
       <c r="D9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="11">
         <v>4</v>
@@ -1228,11 +1327,17 @@
       <c r="D10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="11">
         <v>5</v>
       </c>
@@ -1242,11 +1347,17 @@
       <c r="D11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="12">
         <v>6</v>
       </c>
@@ -1256,11 +1367,17 @@
       <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="12">
         <v>7</v>
       </c>
@@ -1270,11 +1387,17 @@
       <c r="D13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="11">
         <v>8</v>
       </c>
@@ -1284,97 +1407,124 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="11">
         <v>9</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3" cm="1">
+        <f t="array" aca="1" ref="F15" ca="1">F13:F15</f>
+        <v>0</v>
+      </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="12">
         <v>10</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3" cm="1">
+        <f t="array" aca="1" ref="F16" ca="1">F14:F16</f>
+        <v>0</v>
+      </c>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="12">
         <v>11</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="F17" s="3" cm="1">
+        <f t="array" aca="1" ref="F17" ca="1">F15:F17</f>
+        <v>0</v>
+      </c>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="11">
         <v>12</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" cm="1">
+        <f t="array" aca="1" ref="F18" ca="1">F16:F18</f>
+        <v>0</v>
+      </c>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="11">
         <v>13</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="F19" s="3" cm="1">
+        <f t="array" aca="1" ref="F19" ca="1">F17:F19</f>
+        <v>0</v>
+      </c>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="12">
         <v>14</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3" cm="1">
+        <f t="array" aca="1" ref="F20" ca="1">F18:F20</f>
+        <v>0</v>
+      </c>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="12">
         <v>15</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3" cm="1">
+        <f t="array" aca="1" ref="F21" ca="1">F19:F21</f>
+        <v>0</v>
+      </c>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>16</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="F22" s="3" cm="1">
+        <f t="array" aca="1" ref="F22" ca="1">F20:F22</f>
+        <v>0</v>
+      </c>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="11">
         <v>17</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="F23" s="3" cm="1">
+        <f t="array" aca="1" ref="F23" ca="1">F21:F23</f>
+        <v>0</v>
+      </c>
       <c r="G23" s="3"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B25" s="19" t="s">
         <v>6</v>
       </c>

</xml_diff>